<commit_message>
added plotting a simple finction
</commit_message>
<xml_diff>
--- a/lab_first_year/second_semester/rcl_circuits/data.xlsx
+++ b/lab_first_year/second_semester/rcl_circuits/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\PycharmProjects\physics_python_tools\lab_first_year\second_semester\rcl_circuits\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4019EFD4-F9C4-42EB-8A51-32FA0D989317}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616DC4EF-DD7E-4F5B-80BD-9A9140192747}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7575" activeTab="1" xr2:uid="{BD4DC7C5-4D74-48F5-A469-22171841420F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7575" xr2:uid="{BD4DC7C5-4D74-48F5-A469-22171841420F}"/>
   </bookViews>
   <sheets>
     <sheet name="first_phase" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="22">
   <si>
     <t>Resistor</t>
   </si>
@@ -85,6 +85,18 @@
   </si>
   <si>
     <t>freq</t>
+  </si>
+  <si>
+    <t>vr/v0</t>
+  </si>
+  <si>
+    <t>d(vr/v0)</t>
+  </si>
+  <si>
+    <t>d1(dvr/v0)</t>
+  </si>
+  <si>
+    <t>d2(vr*dv0/v0^2)</t>
   </si>
 </sst>
 </file>
@@ -734,20 +746,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9C08235-1664-45A6-916B-2A0524B8D1A3}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:K4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12.5" customWidth="1"/>
     <col min="6" max="6" width="12.5" customWidth="1"/>
-    <col min="10" max="10" width="12.5" customWidth="1"/>
+    <col min="10" max="10" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -765,7 +778,7 @@
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
     </row>
-    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -794,7 +807,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -805,12 +818,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -837,6 +850,36 @@
       </c>
       <c r="I7" t="s">
         <v>16</v>
+      </c>
+      <c r="J7" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" t="s">
+        <v>18</v>
+      </c>
+      <c r="M7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J8" t="e">
+        <f>C8/D8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K8" t="e">
+        <f>B8*E8/(D8^2)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L8" t="e">
+        <f>B8/D8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M8" t="e">
+        <f>SQRT(SUM(J8^2,K8^2))</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
@@ -859,8 +902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FBD1456-7EE7-4E01-91AB-0C486469D68E}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added visualizing stuff. fixed math. added  data
</commit_message>
<xml_diff>
--- a/lab_first_year/second_semester/rcl_circuits/data.xlsx
+++ b/lab_first_year/second_semester/rcl_circuits/data.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\PycharmProjects\physics_python_tools\lab_first_year\second_semester\rcl_circuits\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\PycharmProjects\physics_lab_first_semester\lab_first_year\second_semester\rcl_circuits\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616DC4EF-DD7E-4F5B-80BD-9A9140192747}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7575" xr2:uid="{BD4DC7C5-4D74-48F5-A469-22171841420F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7575"/>
   </bookViews>
   <sheets>
     <sheet name="first_phase" sheetId="1" r:id="rId1"/>
     <sheet name="second_phase" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
   <si>
     <t>Resistor</t>
   </si>
@@ -75,13 +74,7 @@
     <t>phase1</t>
   </si>
   <si>
-    <t>phase2</t>
-  </si>
-  <si>
     <t>dphase1</t>
-  </si>
-  <si>
-    <t>dphase2</t>
   </si>
   <si>
     <t>freq</t>
@@ -98,16 +91,37 @@
   <si>
     <t>d2(vr*dv0/v0^2)</t>
   </si>
+  <si>
+    <t>scop resolution</t>
+  </si>
+  <si>
+    <t>A Volt</t>
+  </si>
+  <si>
+    <t>B Volt</t>
+  </si>
+  <si>
+    <t>omega</t>
+  </si>
+  <si>
+    <t>dpmega</t>
+  </si>
+  <si>
+    <t>1.5nF</t>
+  </si>
+  <si>
+    <t>826.1 mH</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -115,7 +129,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -123,14 +137,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF222222"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF222222"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -194,16 +208,16 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -214,16 +228,16 @@
   <dxfs count="12">
     <dxf>
       <border outline="0">
-        <bottom style="thin">
+        <top style="thin">
           <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
+        </top>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
-        <top style="thin">
+        <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
-        </top>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -240,7 +254,6 @@
         <sz val="11"/>
         <color theme="0"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -252,16 +265,16 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
+        <top style="thin">
           <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
+        </top>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
-        <top style="thin">
+        <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
-        </top>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -278,31 +291,6 @@
         <sz val="11"/>
         <color theme="0"/>
         <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Arial"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -314,16 +302,16 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
+        <top style="thin">
           <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
+        </top>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
-        <top style="thin">
+        <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
-        </top>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -340,7 +328,6 @@
         <sz val="11"/>
         <color theme="0"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -352,17 +339,40 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -378,72 +388,72 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DA32882C-5974-4086-9163-BA19101758AD}" name="טבלה1" displayName="טבלה1" ref="A2:C4" totalsRowShown="0">
-  <autoFilter ref="A2:C4" xr:uid="{7F294251-3B80-4B07-B9F0-1FAC26F0F1D2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="טבלה1" displayName="טבלה1" ref="A2:C4" totalsRowShown="0">
+  <autoFilter ref="A2:C4"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{253B37D6-58C3-4443-A8D4-11D33472C942}" name="type"/>
-    <tableColumn id="2" xr3:uid="{E62F4E41-6620-45A7-9120-817062EC195C}" name="messsured"/>
-    <tableColumn id="3" xr3:uid="{FAB8FE8D-4623-4828-BB6F-1B3F78C99C96}" name="scale"/>
+    <tableColumn id="1" name="type"/>
+    <tableColumn id="2" name="messsured"/>
+    <tableColumn id="3" name="scale"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{205AA75B-D2ED-4E23-9393-54486DD3D6D2}" name="טבלה2" displayName="טבלה2" ref="E2:G4" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="11">
-  <autoFilter ref="E2:G4" xr:uid="{A830DAF1-B7A6-40AC-BC9B-9F7D1887AE7E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="טבלה2" displayName="טבלה2" ref="E2:G4" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9">
+  <autoFilter ref="E2:G4"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{80040B7A-3687-468A-A23F-DA299CDE683E}" name="type"/>
-    <tableColumn id="2" xr3:uid="{C225F6FB-CECF-4039-B2A2-714F91A1FD96}" name="messsured"/>
-    <tableColumn id="3" xr3:uid="{D3BD8FF2-1538-4804-9655-35D71C75F211}" name="scale"/>
+    <tableColumn id="1" name="type"/>
+    <tableColumn id="2" name="messsured"/>
+    <tableColumn id="3" name="scale"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A399818E-96AD-4F58-A6BA-BD3955CC8CBD}" name="טבלה3" displayName="טבלה3" ref="I2:K4" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="8">
-  <autoFilter ref="I2:K4" xr:uid="{0D730968-F837-4CF1-969C-F59D6928D631}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="טבלה3" displayName="טבלה3" ref="I2:K4" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6">
+  <autoFilter ref="I2:K4"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{3AD5D8A1-ADB9-48A4-B33B-59F0C1ECD375}" name="type"/>
-    <tableColumn id="2" xr3:uid="{40F7B9AC-7826-4F5C-97CA-FE3DE0E5700F}" name="messsured"/>
-    <tableColumn id="3" xr3:uid="{3C6B84B0-FF7A-42E8-97EA-00FA91E0B787}" name="scale"/>
+    <tableColumn id="1" name="type"/>
+    <tableColumn id="2" name="messsured"/>
+    <tableColumn id="3" name="scale"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CA42BA42-7F79-4659-A70C-EBC0627914D0}" name="טבלה15" displayName="טבלה15" ref="A2:C4" totalsRowShown="0">
-  <autoFilter ref="A2:C4" xr:uid="{557204FF-1CA5-4760-85CD-A4EEE694DC0C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="טבלה15" displayName="טבלה15" ref="A2:C4" totalsRowShown="0">
+  <autoFilter ref="A2:C4"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{0BA7D1A2-6599-4509-BB3A-5829BD7B0717}" name="type"/>
-    <tableColumn id="2" xr3:uid="{E8CFCD4C-5B79-49DE-8AAE-40D4533790B0}" name="messsured"/>
-    <tableColumn id="3" xr3:uid="{98D58335-A67E-4BE6-85EC-704F8C2F2D8C}" name="scale"/>
+    <tableColumn id="1" name="type"/>
+    <tableColumn id="2" name="messsured"/>
+    <tableColumn id="3" name="scale"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{950C01B6-2CC1-4E71-B0EC-8B104370EB6E}" name="טבלה26" displayName="טבלה26" ref="E2:G4" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="3" tableBorderDxfId="4">
-  <autoFilter ref="E2:G4" xr:uid="{908E4DAE-C895-4989-B57B-9B2B275B5886}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="טבלה26" displayName="טבלה26" ref="E2:G4" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="E2:G4"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{1878A956-4A38-44E7-9475-1DC33CA530FC}" name="type"/>
-    <tableColumn id="2" xr3:uid="{6FFDA97B-7102-4488-AAD2-21CAC0897F3B}" name="messsured"/>
-    <tableColumn id="3" xr3:uid="{09827DEB-201C-4F91-B3E2-D1CA244AFA67}" name="scale"/>
+    <tableColumn id="1" name="type"/>
+    <tableColumn id="2" name="messsured"/>
+    <tableColumn id="3" name="scale"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{79735526-977F-4C23-B780-894A3681BD3B}" name="טבלה37" displayName="טבלה37" ref="I2:K4" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="0" tableBorderDxfId="1">
-  <autoFilter ref="I2:K4" xr:uid="{D1FFF45E-1FD3-466C-ACBF-375EE89ED5D6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="טבלה37" displayName="טבלה37" ref="I2:K4" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
+  <autoFilter ref="I2:K4"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{7FBC4B69-A8B9-47B9-BDCF-5AAD7B065357}" name="type"/>
-    <tableColumn id="2" xr3:uid="{7E509A5B-8DE9-46AE-9D1C-EBCF2A476D82}" name="messsured"/>
-    <tableColumn id="3" xr3:uid="{16796BE5-F478-43A7-8FB5-846A24B06CF9}" name="scale"/>
+    <tableColumn id="1" name="type"/>
+    <tableColumn id="2" name="messsured"/>
+    <tableColumn id="3" name="scale"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -745,40 +755,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9C08235-1664-45A6-916B-2A0524B8D1A3}">
-  <dimension ref="A1:M8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.5" customWidth="1"/>
-    <col min="6" max="6" width="12.5" customWidth="1"/>
-    <col min="10" max="10" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="2" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
       <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
     </row>
-    <row r="2" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -788,44 +799,61 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
+      <c r="B3">
+        <v>6000</v>
+      </c>
       <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -840,46 +868,1795 @@
         <v>12</v>
       </c>
       <c r="F7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" t="s">
+        <v>23</v>
+      </c>
+      <c r="M7" t="s">
+        <v>24</v>
+      </c>
+      <c r="N7" t="s">
         <v>13</v>
       </c>
-      <c r="G7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="O7" t="s">
         <v>14</v>
       </c>
-      <c r="I7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J7" t="s">
-        <v>20</v>
-      </c>
-      <c r="K7" t="s">
-        <v>21</v>
-      </c>
-      <c r="L7" t="s">
-        <v>18</v>
-      </c>
-      <c r="M7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="J8" t="e">
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>430</v>
+      </c>
+      <c r="B8">
+        <v>4.12</v>
+      </c>
+      <c r="C8">
+        <f>B$5/SQRT(12)</f>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="D8">
+        <v>0.17</v>
+      </c>
+      <c r="E8">
+        <f>B$5/SQRT(12)</f>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="F8">
+        <v>0.1</v>
+      </c>
+      <c r="G8">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="H8">
         <f>C8/D8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K8" t="e">
+        <v>1.6980890270283111E-3</v>
+      </c>
+      <c r="I8">
         <f>B8*E8/(D8^2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L8" t="e">
-        <f>B8/D8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M8" t="e">
-        <f>SQRT(SUM(J8^2,K8^2))</f>
-        <v>#DIV/0!</v>
+        <v>4.1153687007980236E-2</v>
+      </c>
+      <c r="J8">
+        <f>D8/B8</f>
+        <v>4.12621359223301E-2</v>
+      </c>
+      <c r="K8">
+        <f>SQRT(SUM(H8^2,I8^2))</f>
+        <v>4.1188705499135503E-2</v>
+      </c>
+      <c r="L8">
+        <f>A8*2*PI()</f>
+        <v>2701.769682087222</v>
+      </c>
+      <c r="M8">
+        <f>2*PI()*0.00005</f>
+        <v>3.1415926535897931E-4</v>
+      </c>
+      <c r="O8" t="e">
+        <f>ASIN(G8/F8)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>530</v>
+      </c>
+      <c r="B9">
+        <v>4.12</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ref="C9:C40" si="0">B$5/SQRT(12)</f>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="D9">
+        <v>0.2</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ref="E9:E40" si="1">B$5/SQRT(12)</f>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="F9">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G9">
+        <v>0.12</v>
+      </c>
+      <c r="H9">
+        <f>C9/D9</f>
+        <v>1.4433756729740645E-3</v>
+      </c>
+      <c r="I9">
+        <f>B9*E9/(D9^2)</f>
+        <v>2.9733538863265723E-2</v>
+      </c>
+      <c r="J9">
+        <f>D9/B9</f>
+        <v>4.8543689320388349E-2</v>
+      </c>
+      <c r="K9">
+        <f t="shared" ref="K9:K40" si="2">SQRT(SUM(H9^2,I9^2))</f>
+        <v>2.976855163871206E-2</v>
+      </c>
+      <c r="L9">
+        <f>A9*2*PI()</f>
+        <v>3330.0882128051808</v>
+      </c>
+      <c r="M9">
+        <f t="shared" ref="M9:M40" si="3">2*PI()*0.00005</f>
+        <v>3.1415926535897931E-4</v>
+      </c>
+      <c r="O9">
+        <f>ASIN(G9/F9)</f>
+        <v>1.0296968008377505</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>830</v>
+      </c>
+      <c r="B10">
+        <v>4.12</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="D10">
+        <v>0.27</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="F10">
+        <v>0.2</v>
+      </c>
+      <c r="G10">
+        <v>0.192</v>
+      </c>
+      <c r="H10">
+        <f>C10/D10</f>
+        <v>1.0691671651659736E-3</v>
+      </c>
+      <c r="I10">
+        <f>B10*E10/(D10^2)</f>
+        <v>1.6314698964754855E-2</v>
+      </c>
+      <c r="J10">
+        <f>D10/B10</f>
+        <v>6.553398058252427E-2</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="2"/>
+        <v>1.6349694820932962E-2</v>
+      </c>
+      <c r="L10">
+        <f>A10*2*PI()</f>
+        <v>5215.0438049590566</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="3"/>
+        <v>3.1415926535897931E-4</v>
+      </c>
+      <c r="O10">
+        <f>ASIN(G10/F10)</f>
+        <v>1.2870022175865685</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1430</v>
+      </c>
+      <c r="B11">
+        <v>4.12</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="D11">
+        <v>0.42</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="F11">
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="G11">
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="H11">
+        <f>C11/D11</f>
+        <v>6.8732174903526888E-4</v>
+      </c>
+      <c r="I11">
+        <f>B11*E11/(D11^2)</f>
+        <v>6.7422990619650184E-3</v>
+      </c>
+      <c r="J11">
+        <f>D11/B11</f>
+        <v>0.10194174757281553</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="2"/>
+        <v>6.7772419041724685E-3</v>
+      </c>
+      <c r="L11">
+        <f>A11*2*PI()</f>
+        <v>8984.9549892668092</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="3"/>
+        <v>3.1415926535897931E-4</v>
+      </c>
+      <c r="O11">
+        <f>ASIN(G11/F11)</f>
+        <v>1.2731996364414639</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1730</v>
+      </c>
+      <c r="B12">
+        <v>4.12</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="D12">
+        <v>0.54400000000000004</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="F12">
+        <v>0.48</v>
+      </c>
+      <c r="G12">
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="H12">
+        <f>C12/D12</f>
+        <v>5.306528209463472E-4</v>
+      </c>
+      <c r="I12">
+        <f>B12*E12/(D12^2)</f>
+        <v>4.0189147468730705E-3</v>
+      </c>
+      <c r="J12">
+        <f>D12/B12</f>
+        <v>0.13203883495145632</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="2"/>
+        <v>4.0537967584737336E-3</v>
+      </c>
+      <c r="L12">
+        <f>A12*2*PI()</f>
+        <v>10869.910581420685</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="3"/>
+        <v>3.1415926535897931E-4</v>
+      </c>
+      <c r="O12">
+        <f>ASIN(G12/F12)</f>
+        <v>1.2035883062370596</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2030</v>
+      </c>
+      <c r="B13">
+        <v>4.12</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="D13">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="F13">
+        <v>0.59199999999999997</v>
+      </c>
+      <c r="G13">
+        <v>0.55200000000000005</v>
+      </c>
+      <c r="H13">
+        <f>C13/D13</f>
+        <v>4.4005355883355624E-4</v>
+      </c>
+      <c r="I13">
+        <f>B13*E13/(D13^2)</f>
+        <v>2.7637510097473345E-3</v>
+      </c>
+      <c r="J13">
+        <f>D13/B13</f>
+        <v>0.15922330097087378</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="2"/>
+        <v>2.7985651285116608E-3</v>
+      </c>
+      <c r="L13">
+        <f>A13*2*PI()</f>
+        <v>12754.866173574561</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="3"/>
+        <v>3.1415926535897931E-4</v>
+      </c>
+      <c r="O13">
+        <f>ASIN(G13/F13)</f>
+        <v>1.2010870395684783</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2330</v>
+      </c>
+      <c r="B14">
+        <v>4.12</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="D14">
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="F14">
+        <v>0.74399999999999999</v>
+      </c>
+      <c r="G14">
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="H14">
+        <f>C14/D14</f>
+        <v>3.6448880630658194E-4</v>
+      </c>
+      <c r="I14">
+        <f>B14*E14/(D14^2)</f>
+        <v>1.8960781338170675E-3</v>
+      </c>
+      <c r="J14">
+        <f>D14/B14</f>
+        <v>0.19223300970873786</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="2"/>
+        <v>1.9307937174804588E-3</v>
+      </c>
+      <c r="L14">
+        <f>A14*2*PI()</f>
+        <v>14639.821765728437</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="3"/>
+        <v>3.1415926535897931E-4</v>
+      </c>
+      <c r="O14">
+        <f>ASIN(G14/F14)</f>
+        <v>1.2413962034273813</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2630</v>
+      </c>
+      <c r="B15">
+        <v>4.12</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="D15">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="F15">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="G15">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="H15">
+        <f>C15/D15</f>
+        <v>2.9100315987380334E-4</v>
+      </c>
+      <c r="I15">
+        <f>B15*E15/(D15^2)</f>
+        <v>1.2086018333468446E-3</v>
+      </c>
+      <c r="J15">
+        <f>D15/B15</f>
+        <v>0.24077669902912621</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="2"/>
+        <v>1.2431416776159878E-3</v>
+      </c>
+      <c r="L15">
+        <f>A15*2*PI()</f>
+        <v>16524.777357882311</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="3"/>
+        <v>3.1415926535897931E-4</v>
+      </c>
+      <c r="O15">
+        <f>ASIN(G15/F15)</f>
+        <v>1.2246229304885385</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2930</v>
+      </c>
+      <c r="B16">
+        <v>4.12</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="D16">
+        <v>1.28</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="F16">
+        <v>1.3</v>
+      </c>
+      <c r="G16">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="H16">
+        <f>C16/D16</f>
+        <v>2.2552744890219758E-4</v>
+      </c>
+      <c r="I16">
+        <f>B16*E16/(D16^2)</f>
+        <v>7.2591647615394836E-4</v>
+      </c>
+      <c r="J16">
+        <f>D16/B16</f>
+        <v>0.31067961165048541</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="2"/>
+        <v>7.6014298691765827E-4</v>
+      </c>
+      <c r="L16">
+        <f>A16*2*PI()</f>
+        <v>18409.732950036188</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="3"/>
+        <v>3.1415926535897931E-4</v>
+      </c>
+      <c r="O16">
+        <f>ASIN(G16/F16)</f>
+        <v>1.0694224805488273</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>3230</v>
+      </c>
+      <c r="B17">
+        <v>4.12</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="D17">
+        <v>1.74</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="F17">
+        <v>1.72</v>
+      </c>
+      <c r="G17">
+        <v>1.48</v>
+      </c>
+      <c r="H17">
+        <f>C17/D17</f>
+        <v>1.6590524976713386E-4</v>
+      </c>
+      <c r="I17">
+        <f>B17*E17/(D17^2)</f>
+        <v>3.9283312013827095E-4</v>
+      </c>
+      <c r="J17">
+        <f>D17/B17</f>
+        <v>0.42233009708737862</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="2"/>
+        <v>4.2642984437989828E-4</v>
+      </c>
+      <c r="L17">
+        <f>A17*2*PI()</f>
+        <v>20294.688542190062</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="3"/>
+        <v>3.1415926535897931E-4</v>
+      </c>
+      <c r="O17">
+        <f>ASIN(G17/F17)</f>
+        <v>1.0361818409474326</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>3530</v>
+      </c>
+      <c r="B18">
+        <v>4.12</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="D18">
+        <v>2.52</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="F18">
+        <v>2.52</v>
+      </c>
+      <c r="G18">
+        <v>1.84</v>
+      </c>
+      <c r="H18">
+        <f>C18/D18</f>
+        <v>1.1455362483921147E-4</v>
+      </c>
+      <c r="I18">
+        <f>B18*E18/(D18^2)</f>
+        <v>1.8728608505458381E-4</v>
+      </c>
+      <c r="J18">
+        <f>D18/B18</f>
+        <v>0.61165048543689315</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="2"/>
+        <v>2.1954181974939447E-4</v>
+      </c>
+      <c r="L18">
+        <f>A18*2*PI()</f>
+        <v>22179.64413434394</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="3"/>
+        <v>3.1415926535897931E-4</v>
+      </c>
+      <c r="O18">
+        <f>ASIN(G18/F18)</f>
+        <v>0.81855422880291495</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>3830</v>
+      </c>
+      <c r="B19">
+        <v>4.12</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="D19">
+        <v>3.52</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="F19">
+        <v>3.52</v>
+      </c>
+      <c r="G19">
+        <v>0.96</v>
+      </c>
+      <c r="H19">
+        <f>C19/D19</f>
+        <v>8.2009981418980935E-5</v>
+      </c>
+      <c r="I19">
+        <f>B19*E19/(D19^2)</f>
+        <v>9.5988955524489058E-5</v>
+      </c>
+      <c r="J19">
+        <f>D19/B19</f>
+        <v>0.85436893203883491</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="2"/>
+        <v>1.2625179854173935E-4</v>
+      </c>
+      <c r="L19">
+        <f>A19*2*PI()</f>
+        <v>24064.599726497814</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="3"/>
+        <v>3.1415926535897931E-4</v>
+      </c>
+      <c r="O19">
+        <f>ASIN(G19/F19)</f>
+        <v>0.27622663076359155</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>4130</v>
+      </c>
+      <c r="B20">
+        <v>4.12</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="D20">
+        <v>3.36</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="F20">
+        <v>3.36</v>
+      </c>
+      <c r="G20">
+        <v>1.48</v>
+      </c>
+      <c r="H20">
+        <f>C20/D20</f>
+        <v>8.591521862940861E-5</v>
+      </c>
+      <c r="I20">
+        <f>B20*E20/(D20^2)</f>
+        <v>1.0534842284320341E-4</v>
+      </c>
+      <c r="J20">
+        <f>D20/B20</f>
+        <v>0.81553398058252424</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="2"/>
+        <v>1.3594011544680056E-4</v>
+      </c>
+      <c r="L20">
+        <f>A20*2*PI()</f>
+        <v>25949.555318651692</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="3"/>
+        <v>3.1415926535897931E-4</v>
+      </c>
+      <c r="O20">
+        <f>ASIN(G20/F20)</f>
+        <v>0.45612902257082272</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>4430</v>
+      </c>
+      <c r="B21">
+        <v>4.12</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="D21">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="F21">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G21">
+        <v>1.8</v>
+      </c>
+      <c r="H21">
+        <f>C21/D21</f>
+        <v>1.2887282794411288E-4</v>
+      </c>
+      <c r="I21">
+        <f>B21*E21/(D21^2)</f>
+        <v>2.3703395139720762E-4</v>
+      </c>
+      <c r="J21">
+        <f>D21/B21</f>
+        <v>0.54368932038834961</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="2"/>
+        <v>2.6980233486255585E-4</v>
+      </c>
+      <c r="L21">
+        <f>A21*2*PI()</f>
+        <v>27834.510910805566</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="3"/>
+        <v>3.1415926535897931E-4</v>
+      </c>
+      <c r="O21">
+        <f>ASIN(G21/F21)</f>
+        <v>0.95824158845555762</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>4730</v>
+      </c>
+      <c r="B22">
+        <v>4.12</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="D22">
+        <v>1.56</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="1"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="F22">
+        <v>1.56</v>
+      </c>
+      <c r="G22">
+        <v>1.28</v>
+      </c>
+      <c r="H22">
+        <f>C22/D22</f>
+        <v>1.8504816320180314E-4</v>
+      </c>
+      <c r="I22">
+        <f>B22*E22/(D22^2)</f>
+        <v>4.8871694384065953E-4</v>
+      </c>
+      <c r="J22">
+        <f>D22/B22</f>
+        <v>0.37864077669902912</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="2"/>
+        <v>5.2257733772267197E-4</v>
+      </c>
+      <c r="L22">
+        <f>A22*2*PI()</f>
+        <v>29719.466502959443</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="3"/>
+        <v>3.1415926535897931E-4</v>
+      </c>
+      <c r="O22">
+        <f>ASIN(G22/F22)</f>
+        <v>0.96230756461053713</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>5030</v>
+      </c>
+      <c r="B23">
+        <v>4.12</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="D23">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="F23">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <f>C23/D23</f>
+        <v>2.5322380227615167E-4</v>
+      </c>
+      <c r="I23">
+        <f>B23*E23/(D23^2)</f>
+        <v>9.1515970647170614E-4</v>
+      </c>
+      <c r="J23">
+        <f>D23/B23</f>
+        <v>0.27669902912621358</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="2"/>
+        <v>9.4954704064020487E-4</v>
+      </c>
+      <c r="L23">
+        <f>A23*2*PI()</f>
+        <v>31604.422095113317</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="3"/>
+        <v>3.1415926535897931E-4</v>
+      </c>
+      <c r="O23">
+        <f>ASIN(G23/F23)</f>
+        <v>1.1036502157860613</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>5330</v>
+      </c>
+      <c r="B24">
+        <v>4.12</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="D24">
+        <v>0.9</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="F24">
+        <v>0.86</v>
+      </c>
+      <c r="G24">
+        <v>0.74</v>
+      </c>
+      <c r="H24">
+        <f>C24/D24</f>
+        <v>3.2075014954979211E-4</v>
+      </c>
+      <c r="I24">
+        <f>B24*E24/(D24^2)</f>
+        <v>1.4683229068279372E-3</v>
+      </c>
+      <c r="J24">
+        <f>D24/B24</f>
+        <v>0.21844660194174756</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="2"/>
+        <v>1.5029480420666102E-3</v>
+      </c>
+      <c r="L24">
+        <f>A24*2*PI()</f>
+        <v>33489.377687267195</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="3"/>
+        <v>3.1415926535897931E-4</v>
+      </c>
+      <c r="O24">
+        <f>ASIN(G24/F24)</f>
+        <v>1.0361818409474326</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>5630</v>
+      </c>
+      <c r="B25">
+        <v>4.12</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="D25">
+        <v>0.7</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="F25">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="G25">
+        <v>0.6</v>
+      </c>
+      <c r="H25">
+        <f>C25/D25</f>
+        <v>4.1239304942116133E-4</v>
+      </c>
+      <c r="I25">
+        <f>B25*E25/(D25^2)</f>
+        <v>2.4272276623074065E-3</v>
+      </c>
+      <c r="J25">
+        <f>D25/B25</f>
+        <v>0.1699029126213592</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="2"/>
+        <v>2.4620118098581823E-3</v>
+      </c>
+      <c r="L25">
+        <f>A25*2*PI()</f>
+        <v>35374.333279421073</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="3"/>
+        <v>3.1415926535897931E-4</v>
+      </c>
+      <c r="O25">
+        <f>ASIN(G25/F25)</f>
+        <v>1.2512151691232347</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>5930</v>
+      </c>
+      <c r="B26">
+        <v>4.12</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="D26">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="1"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="F26">
+        <v>0.504</v>
+      </c>
+      <c r="G26">
+        <v>0.48</v>
+      </c>
+      <c r="H26">
+        <f>C26/D26</f>
+        <v>5.1549131177645153E-4</v>
+      </c>
+      <c r="I26">
+        <f>B26*E26/(D26^2)</f>
+        <v>3.7925432223553219E-3</v>
+      </c>
+      <c r="J26">
+        <f>D26/B26</f>
+        <v>0.1359223300970874</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="2"/>
+        <v>3.82741628072389E-3</v>
+      </c>
+      <c r="L26">
+        <f>A26*2*PI()</f>
+        <v>37259.288871574943</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="3"/>
+        <v>3.1415926535897931E-4</v>
+      </c>
+      <c r="O26">
+        <f>ASIN(G26/F26)</f>
+        <v>1.2609516870532695</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>6230</v>
+      </c>
+      <c r="B27">
+        <v>4.12</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="D27">
+        <v>0.46</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="1"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="F27">
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="G27">
+        <v>0.376</v>
+      </c>
+      <c r="H27">
+        <f>C27/D27</f>
+        <v>6.2755464042350622E-4</v>
+      </c>
+      <c r="I27">
+        <f>B27*E27/(D27^2)</f>
+        <v>5.6207067794453169E-3</v>
+      </c>
+      <c r="J27">
+        <f>D27/B27</f>
+        <v>0.11165048543689321</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="2"/>
+        <v>5.655631664740873E-3</v>
+      </c>
+      <c r="L27">
+        <f>A27*2*PI()</f>
+        <v>39144.244463728821</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="3"/>
+        <v>3.1415926535897931E-4</v>
+      </c>
+      <c r="O27">
+        <f>ASIN(G27/F27)</f>
+        <v>1.2516224009967742</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>6530</v>
+      </c>
+      <c r="B28">
+        <v>4.12</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="D28">
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="1"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="F28">
+        <v>0.312</v>
+      </c>
+      <c r="G28">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="H28">
+        <f>C28/D28</f>
+        <v>8.2009981418980945E-4</v>
+      </c>
+      <c r="I28">
+        <f>B28*E28/(D28^2)</f>
+        <v>9.5988955524489057E-3</v>
+      </c>
+      <c r="J28">
+        <f>D28/B28</f>
+        <v>8.5436893203883493E-2</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="2"/>
+        <v>9.6338652436110776E-3</v>
+      </c>
+      <c r="L28">
+        <f>A28*2*PI()</f>
+        <v>41029.200055882699</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="3"/>
+        <v>3.1415926535897931E-4</v>
+      </c>
+      <c r="O28">
+        <f>ASIN(G28/F28)</f>
+        <v>1.1439029220222632</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>6830</v>
+      </c>
+      <c r="B29">
+        <v>4.12</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="D29">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="1"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="F29">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="G29">
+        <v>0.22</v>
+      </c>
+      <c r="H29">
+        <f>C29/D29</f>
+        <v>1.0093536174643808E-3</v>
+      </c>
+      <c r="I29">
+        <f>B29*E29/(D29^2)</f>
+        <v>1.4540338825011363E-2</v>
+      </c>
+      <c r="J29">
+        <f>D29/B29</f>
+        <v>6.9417475728155334E-2</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="2"/>
+        <v>1.4575330111912432E-2</v>
+      </c>
+      <c r="L29">
+        <f>A29*2*PI()</f>
+        <v>42914.155648036576</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="3"/>
+        <v>3.1415926535897931E-4</v>
+      </c>
+      <c r="O29">
+        <f>ASIN(G29/F29)</f>
+        <v>1.2231316863607218</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>3630</v>
+      </c>
+      <c r="B30">
+        <v>4.12</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="D30">
+        <v>2.86</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="1"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="F30">
+        <v>2.88</v>
+      </c>
+      <c r="G30">
+        <v>1.8</v>
+      </c>
+      <c r="H30">
+        <f>C30/D30</f>
+        <v>1.0093536174643808E-4</v>
+      </c>
+      <c r="I30">
+        <f>B30*E30/(D30^2)</f>
+        <v>1.4540338825011362E-4</v>
+      </c>
+      <c r="J30">
+        <f>D30/B30</f>
+        <v>0.69417475728155331</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="2"/>
+        <v>1.7700308631630579E-4</v>
+      </c>
+      <c r="L30">
+        <f>A30*2*PI()</f>
+        <v>22807.962665061899</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="3"/>
+        <v>3.1415926535897931E-4</v>
+      </c>
+      <c r="O30">
+        <f>ASIN(G30/F30)</f>
+        <v>0.67513153293703165</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>3680</v>
+      </c>
+      <c r="B31">
+        <v>4.12</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="D31">
+        <v>3.06</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="1"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="F31">
+        <v>3.08</v>
+      </c>
+      <c r="G31">
+        <v>1.68</v>
+      </c>
+      <c r="H31">
+        <f>C31/D31</f>
+        <v>9.4338279279350612E-5</v>
+      </c>
+      <c r="I31">
+        <f>B31*E31/(D31^2)</f>
+        <v>1.270175524937662E-4</v>
+      </c>
+      <c r="J31">
+        <f>D31/B31</f>
+        <v>0.74271844660194175</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="2"/>
+        <v>1.5821873965777696E-4</v>
+      </c>
+      <c r="L31">
+        <f>A31*2*PI()</f>
+        <v>23122.121930420879</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="3"/>
+        <v>3.1415926535897931E-4</v>
+      </c>
+      <c r="O31">
+        <f>ASIN(G31/F31)</f>
+        <v>0.57693134523645673</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>3730</v>
+      </c>
+      <c r="B32">
+        <v>4.12</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="D32">
+        <v>3.24</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="1"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="F32">
+        <v>3.28</v>
+      </c>
+      <c r="G32">
+        <v>1.56</v>
+      </c>
+      <c r="H32">
+        <f>C32/D32</f>
+        <v>8.9097263763831134E-5</v>
+      </c>
+      <c r="I32">
+        <f>B32*E32/(D32^2)</f>
+        <v>1.1329652058857538E-4</v>
+      </c>
+      <c r="J32">
+        <f>D32/B32</f>
+        <v>0.78640776699029125</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="2"/>
+        <v>1.4413335487554286E-4</v>
+      </c>
+      <c r="L32">
+        <f>A32*2*PI()</f>
+        <v>23436.281195779855</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="3"/>
+        <v>3.1415926535897931E-4</v>
+      </c>
+      <c r="O32">
+        <f>ASIN(G32/F32)</f>
+        <v>0.49565707724527952</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>4230</v>
+      </c>
+      <c r="B33">
+        <v>4.12</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="D33">
+        <v>2.96</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="1"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="F33">
+        <v>2.96</v>
+      </c>
+      <c r="G33">
+        <v>1.88</v>
+      </c>
+      <c r="H33">
+        <f>C33/D33</f>
+        <v>9.7525383309058416E-5</v>
+      </c>
+      <c r="I33">
+        <f>B33*E33/(D33^2)</f>
+        <v>1.3574479028152724E-4</v>
+      </c>
+      <c r="J33">
+        <f>D33/B33</f>
+        <v>0.71844660194174759</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="2"/>
+        <v>1.671461889429567E-4</v>
+      </c>
+      <c r="L33">
+        <f>A33*2*PI()</f>
+        <v>26577.873849369651</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="3"/>
+        <v>3.1415926535897931E-4</v>
+      </c>
+      <c r="O33">
+        <f>ASIN(G33/F33)</f>
+        <v>0.68818346208019376</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>4280</v>
+      </c>
+      <c r="B34">
+        <v>4.12</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="D34">
+        <v>2.78</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="1"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="F34">
+        <v>2.76</v>
+      </c>
+      <c r="G34">
+        <v>1.84</v>
+      </c>
+      <c r="H34">
+        <f>C34/D34</f>
+        <v>1.0383997647295429E-4</v>
+      </c>
+      <c r="I34">
+        <f>B34*E34/(D34^2)</f>
+        <v>1.5389233923329918E-4</v>
+      </c>
+      <c r="J34">
+        <f>D34/B34</f>
+        <v>0.67475728155339798</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="2"/>
+        <v>1.8564911200595746E-4</v>
+      </c>
+      <c r="L34">
+        <f>A34*2*PI()</f>
+        <v>26892.033114728631</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="3"/>
+        <v>3.1415926535897931E-4</v>
+      </c>
+      <c r="O34">
+        <f>ASIN(G34/F34)</f>
+        <v>0.72972765622696645</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>4330</v>
+      </c>
+      <c r="B35">
+        <v>4.12</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="D35">
+        <v>2.6</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="1"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="F35">
+        <v>2.64</v>
+      </c>
+      <c r="G35">
+        <v>1.88</v>
+      </c>
+      <c r="H35">
+        <f>C35/D35</f>
+        <v>1.1102889792108188E-4</v>
+      </c>
+      <c r="I35">
+        <f>B35*E35/(D35^2)</f>
+        <v>1.7593809978263742E-4</v>
+      </c>
+      <c r="J35">
+        <f>D35/B35</f>
+        <v>0.6310679611650486</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="2"/>
+        <v>2.0804237820380565E-4</v>
+      </c>
+      <c r="L35">
+        <f>A35*2*PI()</f>
+        <v>27206.192380087607</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="3"/>
+        <v>3.1415926535897931E-4</v>
+      </c>
+      <c r="O35">
+        <f>ASIN(G35/F35)</f>
+        <v>0.792515024459304</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>3900</v>
+      </c>
+      <c r="B36">
+        <v>4.12</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="D36">
+        <v>3.7</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="1"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="F36">
+        <v>3.68</v>
+      </c>
+      <c r="G36">
+        <v>0.44</v>
+      </c>
+      <c r="H36">
+        <f>C36/D36</f>
+        <v>7.8020306647246727E-5</v>
+      </c>
+      <c r="I36">
+        <f>B36*E36/(D36^2)</f>
+        <v>8.6876665780177435E-5</v>
+      </c>
+      <c r="J36">
+        <f>D36/B36</f>
+        <v>0.89805825242718451</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="2"/>
+        <v>1.1676781793975198E-4</v>
+      </c>
+      <c r="L36">
+        <f>A36*2*PI()</f>
+        <v>24504.422698000388</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="3"/>
+        <v>3.1415926535897931E-4</v>
+      </c>
+      <c r="O36">
+        <f>ASIN(G36/F36)</f>
+        <v>0.11985194670875002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>3950</v>
+      </c>
+      <c r="B37">
+        <v>4.12</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="D37">
+        <v>3.74</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="1"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="F37">
+        <v>3.76</v>
+      </c>
+      <c r="G37">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="H37">
+        <f>C37/D37</f>
+        <v>7.7185864864923236E-5</v>
+      </c>
+      <c r="I37">
+        <f>B37*E37/(D37^2)</f>
+        <v>8.5028278942107937E-5</v>
+      </c>
+      <c r="J37">
+        <f>D37/B37</f>
+        <v>0.90776699029126218</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="2"/>
+        <v>1.148366925455584E-4</v>
+      </c>
+      <c r="L37">
+        <f>A37*2*PI()</f>
+        <v>24818.581963359367</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="3"/>
+        <v>3.1415926535897931E-4</v>
+      </c>
+      <c r="O37">
+        <f>ASIN(G37/F37)</f>
+        <v>1.9682121802022046E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>4000</v>
+      </c>
+      <c r="B38">
+        <v>4.12</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="D38">
+        <v>3.7</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="1"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="F38">
+        <v>3.68</v>
+      </c>
+      <c r="G38">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="H38">
+        <f>C38/D38</f>
+        <v>7.8020306647246727E-5</v>
+      </c>
+      <c r="I38">
+        <f>B38*E38/(D38^2)</f>
+        <v>8.6876665780177435E-5</v>
+      </c>
+      <c r="J38">
+        <f>D38/B38</f>
+        <v>0.89805825242718451</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="2"/>
+        <v>1.1676781793975198E-4</v>
+      </c>
+      <c r="L38">
+        <f>A38*2*PI()</f>
+        <v>25132.741228718343</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="3"/>
+        <v>3.1415926535897931E-4</v>
+      </c>
+      <c r="O38">
+        <f>ASIN(G38/F38)</f>
+        <v>0.15276743158514852</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>4050</v>
+      </c>
+      <c r="B39">
+        <v>4.12</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="D39">
+        <v>3.6</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="1"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="F39">
+        <v>3.56</v>
+      </c>
+      <c r="G39">
+        <v>1.08</v>
+      </c>
+      <c r="H39">
+        <f>C39/D39</f>
+        <v>8.0187537387448027E-5</v>
+      </c>
+      <c r="I39">
+        <f>B39*E39/(D39^2)</f>
+        <v>9.1770181676746073E-5</v>
+      </c>
+      <c r="J39">
+        <f>D39/B39</f>
+        <v>0.87378640776699024</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="2"/>
+        <v>1.2186799168463537E-4</v>
+      </c>
+      <c r="L39">
+        <f>A39*2*PI()</f>
+        <v>25446.900494077323</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="3"/>
+        <v>3.1415926535897931E-4</v>
+      </c>
+      <c r="O39">
+        <f>ASIN(G39/F39)</f>
+        <v>0.30822817128795654</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>3940</v>
+      </c>
+      <c r="B40">
+        <v>4.12</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="D40">
+        <v>3.76</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="1"/>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="F40">
+        <v>3.76</v>
+      </c>
+      <c r="G40">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="H40">
+        <f>C40/D40</f>
+        <v>7.6775301753939608E-5</v>
+      </c>
+      <c r="I40">
+        <f>B40*E40/(D40^2)</f>
+        <v>8.4126128517614669E-5</v>
+      </c>
+      <c r="J40">
+        <f>D40/B40</f>
+        <v>0.9126213592233009</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="2"/>
+        <v>1.1389316247593928E-4</v>
+      </c>
+      <c r="L40">
+        <f>A40*2*PI()</f>
+        <v>24755.750110287569</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="3"/>
+        <v>3.1415926535897931E-4</v>
+      </c>
+      <c r="O40">
+        <f>ASIN(G40/F40)</f>
+        <v>5.8510972154458343E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L41">
+        <f>MIN(L8:L40)</f>
+        <v>2701.769682087222</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L42">
+        <f>MAX(L8:L40)</f>
+        <v>42914.155648036576</v>
       </c>
     </row>
   </sheetData>
@@ -899,34 +2676,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FBD1456-7EE7-4E01-91AB-0C486469D68E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="2" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
       <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
     </row>
-    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -936,37 +2713,37 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
added function for plotting the data alongside the function
</commit_message>
<xml_diff>
--- a/lab_first_year/second_semester/rcl_circuits/data.xlsx
+++ b/lab_first_year/second_semester/rcl_circuits/data.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\PycharmProjects\physics_lab_first_semester\lab_first_year\second_semester\rcl_circuits\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\PycharmProjects\physics_python_tools\lab_first_year\second_semester\rcl_circuits\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{233BF74C-86B8-479D-ABAD-F940489A4004}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7575"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="first_phase" sheetId="1" r:id="rId1"/>
     <sheet name="second_phase" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -116,12 +117,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -129,7 +130,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -137,14 +138,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF222222"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF222222"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -388,72 +389,72 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="טבלה1" displayName="טבלה1" ref="A2:C4" totalsRowShown="0">
-  <autoFilter ref="A2:C4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="טבלה1" displayName="טבלה1" ref="A2:C4" totalsRowShown="0">
+  <autoFilter ref="A2:C4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="type"/>
-    <tableColumn id="2" name="messsured"/>
-    <tableColumn id="3" name="scale"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="type"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="messsured"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="scale"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="טבלה2" displayName="טבלה2" ref="E2:G4" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9">
-  <autoFilter ref="E2:G4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="טבלה2" displayName="טבלה2" ref="E2:G4" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9">
+  <autoFilter ref="E2:G4" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="type"/>
-    <tableColumn id="2" name="messsured"/>
-    <tableColumn id="3" name="scale"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="type"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="messsured"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="scale"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="טבלה3" displayName="טבלה3" ref="I2:K4" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6">
-  <autoFilter ref="I2:K4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="טבלה3" displayName="טבלה3" ref="I2:K4" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6">
+  <autoFilter ref="I2:K4" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="type"/>
-    <tableColumn id="2" name="messsured"/>
-    <tableColumn id="3" name="scale"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="type"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="messsured"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="scale"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="טבלה15" displayName="טבלה15" ref="A2:C4" totalsRowShown="0">
-  <autoFilter ref="A2:C4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="טבלה15" displayName="טבלה15" ref="A2:C4" totalsRowShown="0">
+  <autoFilter ref="A2:C4" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="type"/>
-    <tableColumn id="2" name="messsured"/>
-    <tableColumn id="3" name="scale"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="type"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="messsured"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="scale"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="טבלה26" displayName="טבלה26" ref="E2:G4" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="E2:G4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="טבלה26" displayName="טבלה26" ref="E2:G4" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="E2:G4" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="type"/>
-    <tableColumn id="2" name="messsured"/>
-    <tableColumn id="3" name="scale"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="type"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="messsured"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="scale"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="טבלה37" displayName="טבלה37" ref="I2:K4" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
-  <autoFilter ref="I2:K4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="טבלה37" displayName="טבלה37" ref="I2:K4" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
+  <autoFilter ref="I2:K4" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="type"/>
-    <tableColumn id="2" name="messsured"/>
-    <tableColumn id="3" name="scale"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="type"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="messsured"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="scale"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -755,23 +756,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
       <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.375" customWidth="1"/>
+    <col min="6" max="6" width="12.375" customWidth="1"/>
+    <col min="10" max="10" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -789,7 +790,7 @@
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -818,7 +819,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -838,12 +839,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -851,7 +852,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -898,7 +899,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>430</v>
       </c>
@@ -923,15 +924,15 @@
         <v>0.11600000000000001</v>
       </c>
       <c r="H8">
-        <f>C8/D8</f>
+        <f t="shared" ref="H8:H40" si="0">C8/D8</f>
         <v>1.6980890270283111E-3</v>
       </c>
       <c r="I8">
-        <f>B8*E8/(D8^2)</f>
+        <f t="shared" ref="I8:I40" si="1">B8*E8/(D8^2)</f>
         <v>4.1153687007980236E-2</v>
       </c>
       <c r="J8">
-        <f>D8/B8</f>
+        <f t="shared" ref="J8:J40" si="2">D8/B8</f>
         <v>4.12621359223301E-2</v>
       </c>
       <c r="K8">
@@ -939,7 +940,7 @@
         <v>4.1188705499135503E-2</v>
       </c>
       <c r="L8">
-        <f>A8*2*PI()</f>
+        <f t="shared" ref="L8:L40" si="3">A8*2*PI()</f>
         <v>2701.769682087222</v>
       </c>
       <c r="M8">
@@ -947,11 +948,11 @@
         <v>3.1415926535897931E-4</v>
       </c>
       <c r="O8" t="e">
-        <f>ASIN(G8/F8)</f>
+        <f t="shared" ref="O8:O40" si="4">ASIN(G8/F8)</f>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>530</v>
       </c>
@@ -959,14 +960,14 @@
         <v>4.12</v>
       </c>
       <c r="C9">
-        <f t="shared" ref="C9:C40" si="0">B$5/SQRT(12)</f>
+        <f t="shared" ref="C9:C40" si="5">B$5/SQRT(12)</f>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="D9">
         <v>0.2</v>
       </c>
       <c r="E9">
-        <f t="shared" ref="E9:E40" si="1">B$5/SQRT(12)</f>
+        <f t="shared" ref="E9:E40" si="6">B$5/SQRT(12)</f>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="F9">
@@ -976,35 +977,35 @@
         <v>0.12</v>
       </c>
       <c r="H9">
-        <f>C9/D9</f>
+        <f t="shared" si="0"/>
         <v>1.4433756729740645E-3</v>
       </c>
       <c r="I9">
-        <f>B9*E9/(D9^2)</f>
+        <f t="shared" si="1"/>
         <v>2.9733538863265723E-2</v>
       </c>
       <c r="J9">
-        <f>D9/B9</f>
+        <f t="shared" si="2"/>
         <v>4.8543689320388349E-2</v>
       </c>
       <c r="K9">
-        <f t="shared" ref="K9:K40" si="2">SQRT(SUM(H9^2,I9^2))</f>
+        <f t="shared" ref="K9:K40" si="7">SQRT(SUM(H9^2,I9^2))</f>
         <v>2.976855163871206E-2</v>
       </c>
       <c r="L9">
-        <f>A9*2*PI()</f>
+        <f t="shared" si="3"/>
         <v>3330.0882128051808</v>
       </c>
       <c r="M9">
-        <f t="shared" ref="M9:M40" si="3">2*PI()*0.00005</f>
+        <f t="shared" ref="M9:M40" si="8">2*PI()*0.00005</f>
         <v>3.1415926535897931E-4</v>
       </c>
       <c r="O9">
-        <f>ASIN(G9/F9)</f>
+        <f t="shared" si="4"/>
         <v>1.0296968008377505</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>830</v>
       </c>
@@ -1012,14 +1013,14 @@
         <v>4.12</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="D10">
         <v>0.27</v>
       </c>
       <c r="E10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="F10">
@@ -1029,35 +1030,35 @@
         <v>0.192</v>
       </c>
       <c r="H10">
-        <f>C10/D10</f>
+        <f t="shared" si="0"/>
         <v>1.0691671651659736E-3</v>
       </c>
       <c r="I10">
-        <f>B10*E10/(D10^2)</f>
+        <f t="shared" si="1"/>
         <v>1.6314698964754855E-2</v>
       </c>
       <c r="J10">
-        <f>D10/B10</f>
+        <f t="shared" si="2"/>
         <v>6.553398058252427E-2</v>
       </c>
       <c r="K10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1.6349694820932962E-2</v>
       </c>
       <c r="L10">
-        <f>A10*2*PI()</f>
+        <f t="shared" si="3"/>
         <v>5215.0438049590566</v>
       </c>
       <c r="M10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.1415926535897931E-4</v>
       </c>
       <c r="O10">
-        <f>ASIN(G10/F10)</f>
+        <f t="shared" si="4"/>
         <v>1.2870022175865685</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1430</v>
       </c>
@@ -1065,14 +1066,14 @@
         <v>4.12</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="D11">
         <v>0.42</v>
       </c>
       <c r="E11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="F11">
@@ -1082,35 +1083,35 @@
         <v>0.34799999999999998</v>
       </c>
       <c r="H11">
-        <f>C11/D11</f>
+        <f t="shared" si="0"/>
         <v>6.8732174903526888E-4</v>
       </c>
       <c r="I11">
-        <f>B11*E11/(D11^2)</f>
+        <f t="shared" si="1"/>
         <v>6.7422990619650184E-3</v>
       </c>
       <c r="J11">
-        <f>D11/B11</f>
+        <f t="shared" si="2"/>
         <v>0.10194174757281553</v>
       </c>
       <c r="K11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>6.7772419041724685E-3</v>
       </c>
       <c r="L11">
-        <f>A11*2*PI()</f>
+        <f t="shared" si="3"/>
         <v>8984.9549892668092</v>
       </c>
       <c r="M11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.1415926535897931E-4</v>
       </c>
       <c r="O11">
-        <f>ASIN(G11/F11)</f>
+        <f t="shared" si="4"/>
         <v>1.2731996364414639</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1730</v>
       </c>
@@ -1118,14 +1119,14 @@
         <v>4.12</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="D12">
         <v>0.54400000000000004</v>
       </c>
       <c r="E12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="F12">
@@ -1135,35 +1136,35 @@
         <v>0.44800000000000001</v>
       </c>
       <c r="H12">
-        <f>C12/D12</f>
+        <f t="shared" si="0"/>
         <v>5.306528209463472E-4</v>
       </c>
       <c r="I12">
-        <f>B12*E12/(D12^2)</f>
+        <f t="shared" si="1"/>
         <v>4.0189147468730705E-3</v>
       </c>
       <c r="J12">
-        <f>D12/B12</f>
+        <f t="shared" si="2"/>
         <v>0.13203883495145632</v>
       </c>
       <c r="K12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>4.0537967584737336E-3</v>
       </c>
       <c r="L12">
-        <f>A12*2*PI()</f>
+        <f t="shared" si="3"/>
         <v>10869.910581420685</v>
       </c>
       <c r="M12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.1415926535897931E-4</v>
       </c>
       <c r="O12">
-        <f>ASIN(G12/F12)</f>
+        <f t="shared" si="4"/>
         <v>1.2035883062370596</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2030</v>
       </c>
@@ -1171,14 +1172,14 @@
         <v>4.12</v>
       </c>
       <c r="C13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="D13">
         <v>0.65600000000000003</v>
       </c>
       <c r="E13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="F13">
@@ -1188,35 +1189,35 @@
         <v>0.55200000000000005</v>
       </c>
       <c r="H13">
-        <f>C13/D13</f>
+        <f t="shared" si="0"/>
         <v>4.4005355883355624E-4</v>
       </c>
       <c r="I13">
-        <f>B13*E13/(D13^2)</f>
+        <f t="shared" si="1"/>
         <v>2.7637510097473345E-3</v>
       </c>
       <c r="J13">
-        <f>D13/B13</f>
+        <f t="shared" si="2"/>
         <v>0.15922330097087378</v>
       </c>
       <c r="K13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>2.7985651285116608E-3</v>
       </c>
       <c r="L13">
-        <f>A13*2*PI()</f>
+        <f t="shared" si="3"/>
         <v>12754.866173574561</v>
       </c>
       <c r="M13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.1415926535897931E-4</v>
       </c>
       <c r="O13">
-        <f>ASIN(G13/F13)</f>
+        <f t="shared" si="4"/>
         <v>1.2010870395684783</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2330</v>
       </c>
@@ -1224,14 +1225,14 @@
         <v>4.12</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="D14">
         <v>0.79200000000000004</v>
       </c>
       <c r="E14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="F14">
@@ -1241,35 +1242,35 @@
         <v>0.70399999999999996</v>
       </c>
       <c r="H14">
-        <f>C14/D14</f>
+        <f t="shared" si="0"/>
         <v>3.6448880630658194E-4</v>
       </c>
       <c r="I14">
-        <f>B14*E14/(D14^2)</f>
+        <f t="shared" si="1"/>
         <v>1.8960781338170675E-3</v>
       </c>
       <c r="J14">
-        <f>D14/B14</f>
+        <f t="shared" si="2"/>
         <v>0.19223300970873786</v>
       </c>
       <c r="K14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1.9307937174804588E-3</v>
       </c>
       <c r="L14">
-        <f>A14*2*PI()</f>
+        <f t="shared" si="3"/>
         <v>14639.821765728437</v>
       </c>
       <c r="M14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.1415926535897931E-4</v>
       </c>
       <c r="O14">
-        <f>ASIN(G14/F14)</f>
+        <f t="shared" si="4"/>
         <v>1.2413962034273813</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2630</v>
       </c>
@@ -1277,14 +1278,14 @@
         <v>4.12</v>
       </c>
       <c r="C15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="D15">
         <v>0.99199999999999999</v>
       </c>
       <c r="E15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="F15">
@@ -1294,35 +1295,35 @@
         <v>0.88800000000000001</v>
       </c>
       <c r="H15">
-        <f>C15/D15</f>
+        <f t="shared" si="0"/>
         <v>2.9100315987380334E-4</v>
       </c>
       <c r="I15">
-        <f>B15*E15/(D15^2)</f>
+        <f t="shared" si="1"/>
         <v>1.2086018333468446E-3</v>
       </c>
       <c r="J15">
-        <f>D15/B15</f>
+        <f t="shared" si="2"/>
         <v>0.24077669902912621</v>
       </c>
       <c r="K15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1.2431416776159878E-3</v>
       </c>
       <c r="L15">
-        <f>A15*2*PI()</f>
+        <f t="shared" si="3"/>
         <v>16524.777357882311</v>
       </c>
       <c r="M15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.1415926535897931E-4</v>
       </c>
       <c r="O15">
-        <f>ASIN(G15/F15)</f>
+        <f t="shared" si="4"/>
         <v>1.2246229304885385</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2930</v>
       </c>
@@ -1330,14 +1331,14 @@
         <v>4.12</v>
       </c>
       <c r="C16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="D16">
         <v>1.28</v>
       </c>
       <c r="E16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="F16">
@@ -1347,35 +1348,35 @@
         <v>1.1399999999999999</v>
       </c>
       <c r="H16">
-        <f>C16/D16</f>
+        <f t="shared" si="0"/>
         <v>2.2552744890219758E-4</v>
       </c>
       <c r="I16">
-        <f>B16*E16/(D16^2)</f>
+        <f t="shared" si="1"/>
         <v>7.2591647615394836E-4</v>
       </c>
       <c r="J16">
-        <f>D16/B16</f>
+        <f t="shared" si="2"/>
         <v>0.31067961165048541</v>
       </c>
       <c r="K16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>7.6014298691765827E-4</v>
       </c>
       <c r="L16">
-        <f>A16*2*PI()</f>
+        <f t="shared" si="3"/>
         <v>18409.732950036188</v>
       </c>
       <c r="M16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.1415926535897931E-4</v>
       </c>
       <c r="O16">
-        <f>ASIN(G16/F16)</f>
+        <f t="shared" si="4"/>
         <v>1.0694224805488273</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>3230</v>
       </c>
@@ -1383,14 +1384,14 @@
         <v>4.12</v>
       </c>
       <c r="C17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="D17">
         <v>1.74</v>
       </c>
       <c r="E17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="F17">
@@ -1400,35 +1401,35 @@
         <v>1.48</v>
       </c>
       <c r="H17">
-        <f>C17/D17</f>
+        <f t="shared" si="0"/>
         <v>1.6590524976713386E-4</v>
       </c>
       <c r="I17">
-        <f>B17*E17/(D17^2)</f>
+        <f t="shared" si="1"/>
         <v>3.9283312013827095E-4</v>
       </c>
       <c r="J17">
-        <f>D17/B17</f>
+        <f t="shared" si="2"/>
         <v>0.42233009708737862</v>
       </c>
       <c r="K17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>4.2642984437989828E-4</v>
       </c>
       <c r="L17">
-        <f>A17*2*PI()</f>
+        <f t="shared" si="3"/>
         <v>20294.688542190062</v>
       </c>
       <c r="M17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.1415926535897931E-4</v>
       </c>
       <c r="O17">
-        <f>ASIN(G17/F17)</f>
+        <f t="shared" si="4"/>
         <v>1.0361818409474326</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>3530</v>
       </c>
@@ -1436,14 +1437,14 @@
         <v>4.12</v>
       </c>
       <c r="C18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="D18">
         <v>2.52</v>
       </c>
       <c r="E18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="F18">
@@ -1453,35 +1454,35 @@
         <v>1.84</v>
       </c>
       <c r="H18">
-        <f>C18/D18</f>
+        <f t="shared" si="0"/>
         <v>1.1455362483921147E-4</v>
       </c>
       <c r="I18">
-        <f>B18*E18/(D18^2)</f>
+        <f t="shared" si="1"/>
         <v>1.8728608505458381E-4</v>
       </c>
       <c r="J18">
-        <f>D18/B18</f>
+        <f t="shared" si="2"/>
         <v>0.61165048543689315</v>
       </c>
       <c r="K18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>2.1954181974939447E-4</v>
       </c>
       <c r="L18">
-        <f>A18*2*PI()</f>
+        <f t="shared" si="3"/>
         <v>22179.64413434394</v>
       </c>
       <c r="M18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.1415926535897931E-4</v>
       </c>
       <c r="O18">
-        <f>ASIN(G18/F18)</f>
+        <f t="shared" si="4"/>
         <v>0.81855422880291495</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>3830</v>
       </c>
@@ -1489,14 +1490,14 @@
         <v>4.12</v>
       </c>
       <c r="C19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="D19">
         <v>3.52</v>
       </c>
       <c r="E19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="F19">
@@ -1506,35 +1507,35 @@
         <v>0.96</v>
       </c>
       <c r="H19">
-        <f>C19/D19</f>
+        <f t="shared" si="0"/>
         <v>8.2009981418980935E-5</v>
       </c>
       <c r="I19">
-        <f>B19*E19/(D19^2)</f>
+        <f t="shared" si="1"/>
         <v>9.5988955524489058E-5</v>
       </c>
       <c r="J19">
-        <f>D19/B19</f>
+        <f t="shared" si="2"/>
         <v>0.85436893203883491</v>
       </c>
       <c r="K19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1.2625179854173935E-4</v>
       </c>
       <c r="L19">
-        <f>A19*2*PI()</f>
+        <f t="shared" si="3"/>
         <v>24064.599726497814</v>
       </c>
       <c r="M19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.1415926535897931E-4</v>
       </c>
       <c r="O19">
-        <f>ASIN(G19/F19)</f>
+        <f t="shared" si="4"/>
         <v>0.27622663076359155</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>4130</v>
       </c>
@@ -1542,14 +1543,14 @@
         <v>4.12</v>
       </c>
       <c r="C20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="D20">
         <v>3.36</v>
       </c>
       <c r="E20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="F20">
@@ -1559,35 +1560,35 @@
         <v>1.48</v>
       </c>
       <c r="H20">
-        <f>C20/D20</f>
+        <f t="shared" si="0"/>
         <v>8.591521862940861E-5</v>
       </c>
       <c r="I20">
-        <f>B20*E20/(D20^2)</f>
+        <f t="shared" si="1"/>
         <v>1.0534842284320341E-4</v>
       </c>
       <c r="J20">
-        <f>D20/B20</f>
+        <f t="shared" si="2"/>
         <v>0.81553398058252424</v>
       </c>
       <c r="K20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1.3594011544680056E-4</v>
       </c>
       <c r="L20">
-        <f>A20*2*PI()</f>
+        <f t="shared" si="3"/>
         <v>25949.555318651692</v>
       </c>
       <c r="M20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.1415926535897931E-4</v>
       </c>
       <c r="O20">
-        <f>ASIN(G20/F20)</f>
+        <f t="shared" si="4"/>
         <v>0.45612902257082272</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>4430</v>
       </c>
@@ -1595,14 +1596,14 @@
         <v>4.12</v>
       </c>
       <c r="C21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="D21">
         <v>2.2400000000000002</v>
       </c>
       <c r="E21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="F21">
@@ -1612,35 +1613,35 @@
         <v>1.8</v>
       </c>
       <c r="H21">
-        <f>C21/D21</f>
+        <f t="shared" si="0"/>
         <v>1.2887282794411288E-4</v>
       </c>
       <c r="I21">
-        <f>B21*E21/(D21^2)</f>
+        <f t="shared" si="1"/>
         <v>2.3703395139720762E-4</v>
       </c>
       <c r="J21">
-        <f>D21/B21</f>
+        <f t="shared" si="2"/>
         <v>0.54368932038834961</v>
       </c>
       <c r="K21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>2.6980233486255585E-4</v>
       </c>
       <c r="L21">
-        <f>A21*2*PI()</f>
+        <f t="shared" si="3"/>
         <v>27834.510910805566</v>
       </c>
       <c r="M21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.1415926535897931E-4</v>
       </c>
       <c r="O21">
-        <f>ASIN(G21/F21)</f>
+        <f t="shared" si="4"/>
         <v>0.95824158845555762</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>4730</v>
       </c>
@@ -1648,14 +1649,14 @@
         <v>4.12</v>
       </c>
       <c r="C22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="D22">
         <v>1.56</v>
       </c>
       <c r="E22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="F22">
@@ -1665,35 +1666,35 @@
         <v>1.28</v>
       </c>
       <c r="H22">
-        <f>C22/D22</f>
+        <f t="shared" si="0"/>
         <v>1.8504816320180314E-4</v>
       </c>
       <c r="I22">
-        <f>B22*E22/(D22^2)</f>
+        <f t="shared" si="1"/>
         <v>4.8871694384065953E-4</v>
       </c>
       <c r="J22">
-        <f>D22/B22</f>
+        <f t="shared" si="2"/>
         <v>0.37864077669902912</v>
       </c>
       <c r="K22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>5.2257733772267197E-4</v>
       </c>
       <c r="L22">
-        <f>A22*2*PI()</f>
+        <f t="shared" si="3"/>
         <v>29719.466502959443</v>
       </c>
       <c r="M22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.1415926535897931E-4</v>
       </c>
       <c r="O22">
-        <f>ASIN(G22/F22)</f>
+        <f t="shared" si="4"/>
         <v>0.96230756461053713</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>5030</v>
       </c>
@@ -1701,14 +1702,14 @@
         <v>4.12</v>
       </c>
       <c r="C23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="D23">
         <v>1.1399999999999999</v>
       </c>
       <c r="E23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="F23">
@@ -1718,35 +1719,35 @@
         <v>1</v>
       </c>
       <c r="H23">
-        <f>C23/D23</f>
+        <f t="shared" si="0"/>
         <v>2.5322380227615167E-4</v>
       </c>
       <c r="I23">
-        <f>B23*E23/(D23^2)</f>
+        <f t="shared" si="1"/>
         <v>9.1515970647170614E-4</v>
       </c>
       <c r="J23">
-        <f>D23/B23</f>
+        <f t="shared" si="2"/>
         <v>0.27669902912621358</v>
       </c>
       <c r="K23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>9.4954704064020487E-4</v>
       </c>
       <c r="L23">
-        <f>A23*2*PI()</f>
+        <f t="shared" si="3"/>
         <v>31604.422095113317</v>
       </c>
       <c r="M23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.1415926535897931E-4</v>
       </c>
       <c r="O23">
-        <f>ASIN(G23/F23)</f>
+        <f t="shared" si="4"/>
         <v>1.1036502157860613</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>5330</v>
       </c>
@@ -1754,14 +1755,14 @@
         <v>4.12</v>
       </c>
       <c r="C24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="D24">
         <v>0.9</v>
       </c>
       <c r="E24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="F24">
@@ -1771,35 +1772,35 @@
         <v>0.74</v>
       </c>
       <c r="H24">
-        <f>C24/D24</f>
+        <f t="shared" si="0"/>
         <v>3.2075014954979211E-4</v>
       </c>
       <c r="I24">
-        <f>B24*E24/(D24^2)</f>
+        <f t="shared" si="1"/>
         <v>1.4683229068279372E-3</v>
       </c>
       <c r="J24">
-        <f>D24/B24</f>
+        <f t="shared" si="2"/>
         <v>0.21844660194174756</v>
       </c>
       <c r="K24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1.5029480420666102E-3</v>
       </c>
       <c r="L24">
-        <f>A24*2*PI()</f>
+        <f t="shared" si="3"/>
         <v>33489.377687267195</v>
       </c>
       <c r="M24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.1415926535897931E-4</v>
       </c>
       <c r="O24">
-        <f>ASIN(G24/F24)</f>
+        <f t="shared" si="4"/>
         <v>1.0361818409474326</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>5630</v>
       </c>
@@ -1807,14 +1808,14 @@
         <v>4.12</v>
       </c>
       <c r="C25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="D25">
         <v>0.7</v>
       </c>
       <c r="E25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="F25">
@@ -1824,35 +1825,35 @@
         <v>0.6</v>
       </c>
       <c r="H25">
-        <f>C25/D25</f>
+        <f t="shared" si="0"/>
         <v>4.1239304942116133E-4</v>
       </c>
       <c r="I25">
-        <f>B25*E25/(D25^2)</f>
+        <f t="shared" si="1"/>
         <v>2.4272276623074065E-3</v>
       </c>
       <c r="J25">
-        <f>D25/B25</f>
+        <f t="shared" si="2"/>
         <v>0.1699029126213592</v>
       </c>
       <c r="K25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>2.4620118098581823E-3</v>
       </c>
       <c r="L25">
-        <f>A25*2*PI()</f>
+        <f t="shared" si="3"/>
         <v>35374.333279421073</v>
       </c>
       <c r="M25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.1415926535897931E-4</v>
       </c>
       <c r="O25">
-        <f>ASIN(G25/F25)</f>
+        <f t="shared" si="4"/>
         <v>1.2512151691232347</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>5930</v>
       </c>
@@ -1860,14 +1861,14 @@
         <v>4.12</v>
       </c>
       <c r="C26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="D26">
         <v>0.56000000000000005</v>
       </c>
       <c r="E26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="F26">
@@ -1877,35 +1878,35 @@
         <v>0.48</v>
       </c>
       <c r="H26">
-        <f>C26/D26</f>
+        <f t="shared" si="0"/>
         <v>5.1549131177645153E-4</v>
       </c>
       <c r="I26">
-        <f>B26*E26/(D26^2)</f>
+        <f t="shared" si="1"/>
         <v>3.7925432223553219E-3</v>
       </c>
       <c r="J26">
-        <f>D26/B26</f>
+        <f t="shared" si="2"/>
         <v>0.1359223300970874</v>
       </c>
       <c r="K26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>3.82741628072389E-3</v>
       </c>
       <c r="L26">
-        <f>A26*2*PI()</f>
+        <f t="shared" si="3"/>
         <v>37259.288871574943</v>
       </c>
       <c r="M26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.1415926535897931E-4</v>
       </c>
       <c r="O26">
-        <f>ASIN(G26/F26)</f>
+        <f t="shared" si="4"/>
         <v>1.2609516870532695</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>6230</v>
       </c>
@@ -1913,14 +1914,14 @@
         <v>4.12</v>
       </c>
       <c r="C27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="D27">
         <v>0.46</v>
       </c>
       <c r="E27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="F27">
@@ -1930,35 +1931,35 @@
         <v>0.376</v>
       </c>
       <c r="H27">
-        <f>C27/D27</f>
+        <f t="shared" si="0"/>
         <v>6.2755464042350622E-4</v>
       </c>
       <c r="I27">
-        <f>B27*E27/(D27^2)</f>
+        <f t="shared" si="1"/>
         <v>5.6207067794453169E-3</v>
       </c>
       <c r="J27">
-        <f>D27/B27</f>
+        <f t="shared" si="2"/>
         <v>0.11165048543689321</v>
       </c>
       <c r="K27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>5.655631664740873E-3</v>
       </c>
       <c r="L27">
-        <f>A27*2*PI()</f>
+        <f t="shared" si="3"/>
         <v>39144.244463728821</v>
       </c>
       <c r="M27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.1415926535897931E-4</v>
       </c>
       <c r="O27">
-        <f>ASIN(G27/F27)</f>
+        <f t="shared" si="4"/>
         <v>1.2516224009967742</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>6530</v>
       </c>
@@ -1966,14 +1967,14 @@
         <v>4.12</v>
       </c>
       <c r="C28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="D28">
         <v>0.35199999999999998</v>
       </c>
       <c r="E28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="F28">
@@ -1983,35 +1984,35 @@
         <v>0.28399999999999997</v>
       </c>
       <c r="H28">
-        <f>C28/D28</f>
+        <f t="shared" si="0"/>
         <v>8.2009981418980945E-4</v>
       </c>
       <c r="I28">
-        <f>B28*E28/(D28^2)</f>
+        <f t="shared" si="1"/>
         <v>9.5988955524489057E-3</v>
       </c>
       <c r="J28">
-        <f>D28/B28</f>
+        <f t="shared" si="2"/>
         <v>8.5436893203883493E-2</v>
       </c>
       <c r="K28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>9.6338652436110776E-3</v>
       </c>
       <c r="L28">
-        <f>A28*2*PI()</f>
+        <f t="shared" si="3"/>
         <v>41029.200055882699</v>
       </c>
       <c r="M28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.1415926535897931E-4</v>
       </c>
       <c r="O28">
-        <f>ASIN(G28/F28)</f>
+        <f t="shared" si="4"/>
         <v>1.1439029220222632</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>6830</v>
       </c>
@@ -2019,14 +2020,14 @@
         <v>4.12</v>
       </c>
       <c r="C29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="D29">
         <v>0.28599999999999998</v>
       </c>
       <c r="E29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="F29">
@@ -2036,35 +2037,35 @@
         <v>0.22</v>
       </c>
       <c r="H29">
-        <f>C29/D29</f>
+        <f t="shared" si="0"/>
         <v>1.0093536174643808E-3</v>
       </c>
       <c r="I29">
-        <f>B29*E29/(D29^2)</f>
+        <f t="shared" si="1"/>
         <v>1.4540338825011363E-2</v>
       </c>
       <c r="J29">
-        <f>D29/B29</f>
+        <f t="shared" si="2"/>
         <v>6.9417475728155334E-2</v>
       </c>
       <c r="K29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1.4575330111912432E-2</v>
       </c>
       <c r="L29">
-        <f>A29*2*PI()</f>
+        <f t="shared" si="3"/>
         <v>42914.155648036576</v>
       </c>
       <c r="M29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.1415926535897931E-4</v>
       </c>
       <c r="O29">
-        <f>ASIN(G29/F29)</f>
+        <f t="shared" si="4"/>
         <v>1.2231316863607218</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>3630</v>
       </c>
@@ -2072,14 +2073,14 @@
         <v>4.12</v>
       </c>
       <c r="C30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="D30">
         <v>2.86</v>
       </c>
       <c r="E30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="F30">
@@ -2089,35 +2090,35 @@
         <v>1.8</v>
       </c>
       <c r="H30">
-        <f>C30/D30</f>
+        <f t="shared" si="0"/>
         <v>1.0093536174643808E-4</v>
       </c>
       <c r="I30">
-        <f>B30*E30/(D30^2)</f>
+        <f t="shared" si="1"/>
         <v>1.4540338825011362E-4</v>
       </c>
       <c r="J30">
-        <f>D30/B30</f>
+        <f t="shared" si="2"/>
         <v>0.69417475728155331</v>
       </c>
       <c r="K30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1.7700308631630579E-4</v>
       </c>
       <c r="L30">
-        <f>A30*2*PI()</f>
+        <f t="shared" si="3"/>
         <v>22807.962665061899</v>
       </c>
       <c r="M30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.1415926535897931E-4</v>
       </c>
       <c r="O30">
-        <f>ASIN(G30/F30)</f>
+        <f t="shared" si="4"/>
         <v>0.67513153293703165</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>3680</v>
       </c>
@@ -2125,14 +2126,14 @@
         <v>4.12</v>
       </c>
       <c r="C31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="D31">
         <v>3.06</v>
       </c>
       <c r="E31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="F31">
@@ -2142,35 +2143,35 @@
         <v>1.68</v>
       </c>
       <c r="H31">
-        <f>C31/D31</f>
+        <f t="shared" si="0"/>
         <v>9.4338279279350612E-5</v>
       </c>
       <c r="I31">
-        <f>B31*E31/(D31^2)</f>
+        <f t="shared" si="1"/>
         <v>1.270175524937662E-4</v>
       </c>
       <c r="J31">
-        <f>D31/B31</f>
+        <f t="shared" si="2"/>
         <v>0.74271844660194175</v>
       </c>
       <c r="K31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1.5821873965777696E-4</v>
       </c>
       <c r="L31">
-        <f>A31*2*PI()</f>
+        <f t="shared" si="3"/>
         <v>23122.121930420879</v>
       </c>
       <c r="M31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.1415926535897931E-4</v>
       </c>
       <c r="O31">
-        <f>ASIN(G31/F31)</f>
+        <f t="shared" si="4"/>
         <v>0.57693134523645673</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>3730</v>
       </c>
@@ -2178,14 +2179,14 @@
         <v>4.12</v>
       </c>
       <c r="C32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="D32">
         <v>3.24</v>
       </c>
       <c r="E32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="F32">
@@ -2195,35 +2196,35 @@
         <v>1.56</v>
       </c>
       <c r="H32">
-        <f>C32/D32</f>
+        <f t="shared" si="0"/>
         <v>8.9097263763831134E-5</v>
       </c>
       <c r="I32">
-        <f>B32*E32/(D32^2)</f>
+        <f t="shared" si="1"/>
         <v>1.1329652058857538E-4</v>
       </c>
       <c r="J32">
-        <f>D32/B32</f>
+        <f t="shared" si="2"/>
         <v>0.78640776699029125</v>
       </c>
       <c r="K32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1.4413335487554286E-4</v>
       </c>
       <c r="L32">
-        <f>A32*2*PI()</f>
+        <f t="shared" si="3"/>
         <v>23436.281195779855</v>
       </c>
       <c r="M32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.1415926535897931E-4</v>
       </c>
       <c r="O32">
-        <f>ASIN(G32/F32)</f>
+        <f t="shared" si="4"/>
         <v>0.49565707724527952</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>4230</v>
       </c>
@@ -2231,14 +2232,14 @@
         <v>4.12</v>
       </c>
       <c r="C33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="D33">
         <v>2.96</v>
       </c>
       <c r="E33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="F33">
@@ -2248,35 +2249,35 @@
         <v>1.88</v>
       </c>
       <c r="H33">
-        <f>C33/D33</f>
+        <f t="shared" si="0"/>
         <v>9.7525383309058416E-5</v>
       </c>
       <c r="I33">
-        <f>B33*E33/(D33^2)</f>
+        <f t="shared" si="1"/>
         <v>1.3574479028152724E-4</v>
       </c>
       <c r="J33">
-        <f>D33/B33</f>
+        <f t="shared" si="2"/>
         <v>0.71844660194174759</v>
       </c>
       <c r="K33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1.671461889429567E-4</v>
       </c>
       <c r="L33">
-        <f>A33*2*PI()</f>
+        <f t="shared" si="3"/>
         <v>26577.873849369651</v>
       </c>
       <c r="M33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.1415926535897931E-4</v>
       </c>
       <c r="O33">
-        <f>ASIN(G33/F33)</f>
+        <f t="shared" si="4"/>
         <v>0.68818346208019376</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>4280</v>
       </c>
@@ -2284,14 +2285,14 @@
         <v>4.12</v>
       </c>
       <c r="C34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="D34">
         <v>2.78</v>
       </c>
       <c r="E34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="F34">
@@ -2301,35 +2302,35 @@
         <v>1.84</v>
       </c>
       <c r="H34">
-        <f>C34/D34</f>
+        <f t="shared" si="0"/>
         <v>1.0383997647295429E-4</v>
       </c>
       <c r="I34">
-        <f>B34*E34/(D34^2)</f>
+        <f t="shared" si="1"/>
         <v>1.5389233923329918E-4</v>
       </c>
       <c r="J34">
-        <f>D34/B34</f>
+        <f t="shared" si="2"/>
         <v>0.67475728155339798</v>
       </c>
       <c r="K34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1.8564911200595746E-4</v>
       </c>
       <c r="L34">
-        <f>A34*2*PI()</f>
+        <f t="shared" si="3"/>
         <v>26892.033114728631</v>
       </c>
       <c r="M34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.1415926535897931E-4</v>
       </c>
       <c r="O34">
-        <f>ASIN(G34/F34)</f>
+        <f t="shared" si="4"/>
         <v>0.72972765622696645</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>4330</v>
       </c>
@@ -2337,14 +2338,14 @@
         <v>4.12</v>
       </c>
       <c r="C35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="D35">
         <v>2.6</v>
       </c>
       <c r="E35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="F35">
@@ -2354,35 +2355,35 @@
         <v>1.88</v>
       </c>
       <c r="H35">
-        <f>C35/D35</f>
+        <f t="shared" si="0"/>
         <v>1.1102889792108188E-4</v>
       </c>
       <c r="I35">
-        <f>B35*E35/(D35^2)</f>
+        <f t="shared" si="1"/>
         <v>1.7593809978263742E-4</v>
       </c>
       <c r="J35">
-        <f>D35/B35</f>
+        <f t="shared" si="2"/>
         <v>0.6310679611650486</v>
       </c>
       <c r="K35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>2.0804237820380565E-4</v>
       </c>
       <c r="L35">
-        <f>A35*2*PI()</f>
+        <f t="shared" si="3"/>
         <v>27206.192380087607</v>
       </c>
       <c r="M35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.1415926535897931E-4</v>
       </c>
       <c r="O35">
-        <f>ASIN(G35/F35)</f>
+        <f t="shared" si="4"/>
         <v>0.792515024459304</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>3900</v>
       </c>
@@ -2390,14 +2391,14 @@
         <v>4.12</v>
       </c>
       <c r="C36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="D36">
         <v>3.7</v>
       </c>
       <c r="E36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="F36">
@@ -2407,35 +2408,35 @@
         <v>0.44</v>
       </c>
       <c r="H36">
-        <f>C36/D36</f>
+        <f t="shared" si="0"/>
         <v>7.8020306647246727E-5</v>
       </c>
       <c r="I36">
-        <f>B36*E36/(D36^2)</f>
+        <f t="shared" si="1"/>
         <v>8.6876665780177435E-5</v>
       </c>
       <c r="J36">
-        <f>D36/B36</f>
+        <f t="shared" si="2"/>
         <v>0.89805825242718451</v>
       </c>
       <c r="K36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1.1676781793975198E-4</v>
       </c>
       <c r="L36">
-        <f>A36*2*PI()</f>
+        <f t="shared" si="3"/>
         <v>24504.422698000388</v>
       </c>
       <c r="M36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.1415926535897931E-4</v>
       </c>
       <c r="O36">
-        <f>ASIN(G36/F36)</f>
+        <f t="shared" si="4"/>
         <v>0.11985194670875002</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>3950</v>
       </c>
@@ -2443,14 +2444,14 @@
         <v>4.12</v>
       </c>
       <c r="C37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="D37">
         <v>3.74</v>
       </c>
       <c r="E37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="F37">
@@ -2460,35 +2461,35 @@
         <v>7.3999999999999996E-2</v>
       </c>
       <c r="H37">
-        <f>C37/D37</f>
+        <f t="shared" si="0"/>
         <v>7.7185864864923236E-5</v>
       </c>
       <c r="I37">
-        <f>B37*E37/(D37^2)</f>
+        <f t="shared" si="1"/>
         <v>8.5028278942107937E-5</v>
       </c>
       <c r="J37">
-        <f>D37/B37</f>
+        <f t="shared" si="2"/>
         <v>0.90776699029126218</v>
       </c>
       <c r="K37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1.148366925455584E-4</v>
       </c>
       <c r="L37">
-        <f>A37*2*PI()</f>
+        <f t="shared" si="3"/>
         <v>24818.581963359367</v>
       </c>
       <c r="M37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.1415926535897931E-4</v>
       </c>
       <c r="O37">
-        <f>ASIN(G37/F37)</f>
+        <f t="shared" si="4"/>
         <v>1.9682121802022046E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>4000</v>
       </c>
@@ -2496,14 +2497,14 @@
         <v>4.12</v>
       </c>
       <c r="C38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="D38">
         <v>3.7</v>
       </c>
       <c r="E38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="F38">
@@ -2513,35 +2514,35 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="H38">
-        <f>C38/D38</f>
+        <f t="shared" si="0"/>
         <v>7.8020306647246727E-5</v>
       </c>
       <c r="I38">
-        <f>B38*E38/(D38^2)</f>
+        <f t="shared" si="1"/>
         <v>8.6876665780177435E-5</v>
       </c>
       <c r="J38">
-        <f>D38/B38</f>
+        <f t="shared" si="2"/>
         <v>0.89805825242718451</v>
       </c>
       <c r="K38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1.1676781793975198E-4</v>
       </c>
       <c r="L38">
-        <f>A38*2*PI()</f>
+        <f t="shared" si="3"/>
         <v>25132.741228718343</v>
       </c>
       <c r="M38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.1415926535897931E-4</v>
       </c>
       <c r="O38">
-        <f>ASIN(G38/F38)</f>
+        <f t="shared" si="4"/>
         <v>0.15276743158514852</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>4050</v>
       </c>
@@ -2549,14 +2550,14 @@
         <v>4.12</v>
       </c>
       <c r="C39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="D39">
         <v>3.6</v>
       </c>
       <c r="E39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="F39">
@@ -2566,35 +2567,35 @@
         <v>1.08</v>
       </c>
       <c r="H39">
-        <f>C39/D39</f>
+        <f t="shared" si="0"/>
         <v>8.0187537387448027E-5</v>
       </c>
       <c r="I39">
-        <f>B39*E39/(D39^2)</f>
+        <f t="shared" si="1"/>
         <v>9.1770181676746073E-5</v>
       </c>
       <c r="J39">
-        <f>D39/B39</f>
+        <f t="shared" si="2"/>
         <v>0.87378640776699024</v>
       </c>
       <c r="K39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1.2186799168463537E-4</v>
       </c>
       <c r="L39">
-        <f>A39*2*PI()</f>
+        <f t="shared" si="3"/>
         <v>25446.900494077323</v>
       </c>
       <c r="M39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.1415926535897931E-4</v>
       </c>
       <c r="O39">
-        <f>ASIN(G39/F39)</f>
+        <f t="shared" si="4"/>
         <v>0.30822817128795654</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>3940</v>
       </c>
@@ -2602,14 +2603,14 @@
         <v>4.12</v>
       </c>
       <c r="C40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="D40">
         <v>3.76</v>
       </c>
       <c r="E40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.886751345948129E-4</v>
       </c>
       <c r="F40">
@@ -2619,41 +2620,41 @@
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="H40">
-        <f>C40/D40</f>
+        <f t="shared" si="0"/>
         <v>7.6775301753939608E-5</v>
       </c>
       <c r="I40">
-        <f>B40*E40/(D40^2)</f>
+        <f t="shared" si="1"/>
         <v>8.4126128517614669E-5</v>
       </c>
       <c r="J40">
-        <f>D40/B40</f>
+        <f t="shared" si="2"/>
         <v>0.9126213592233009</v>
       </c>
       <c r="K40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1.1389316247593928E-4</v>
       </c>
       <c r="L40">
-        <f>A40*2*PI()</f>
+        <f t="shared" si="3"/>
         <v>24755.750110287569</v>
       </c>
       <c r="M40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.1415926535897931E-4</v>
       </c>
       <c r="O40">
-        <f>ASIN(G40/F40)</f>
+        <f t="shared" si="4"/>
         <v>5.8510972154458343E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="L41">
         <f>MIN(L8:L40)</f>
         <v>2701.769682087222</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="L42">
         <f>MAX(L8:L40)</f>
         <v>42914.155648036576</v>
@@ -2676,16 +2677,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -2703,7 +2704,7 @@
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2732,7 +2733,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2743,7 +2744,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>

</xml_diff>